<commit_message>
A bit of work
</commit_message>
<xml_diff>
--- a/UniPD/Tutor Didattico/Automi - Semestre 2/Calendario_ALF_2024_Aggiornato_Tutorati.xlsx
+++ b/UniPD/Tutor Didattico/Automi - Semestre 2/Calendario_ALF_2024_Aggiornato_Tutorati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roves\OneDrive\Documenti\GitHub\Teaching-And-Tutoring\UniPD\Tutor Didattico\Automi - Semestre 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722F35A6-FB4B-4901-964C-115C641A26B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FE475B-91E7-41CC-95D6-934629BD5C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7C55FAAF-9703-2848-805D-6B612CD4CF68}"/>
   </bookViews>
@@ -240,9 +240,6 @@
     <t>Esercizi grammatiche CF e automi a pila</t>
   </si>
   <si>
-    <t>Tutorato 5 19/04</t>
-  </si>
-  <si>
     <t>Esercizi primo compitino + pumping lemma CFL</t>
   </si>
   <si>
@@ -270,9 +267,6 @@
     <t>Classi P/NP, Riduzioni + esercizi</t>
   </si>
   <si>
-    <t>Tutorato 10 06/06</t>
-  </si>
-  <si>
     <t>Problemi notevoli P/NP + esercizi secondo compitino</t>
   </si>
   <si>
@@ -283,6 +277,12 @@
   </si>
   <si>
     <t>Aula possibile: Luf2 / 1BC50</t>
+  </si>
+  <si>
+    <t>Tutorato 10 07/06</t>
+  </si>
+  <si>
+    <t>Tutorato 5 18/04</t>
   </si>
 </sst>
 </file>
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B68855-53FD-474B-AE0F-2554AA20AC8B}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -892,7 +892,7 @@
       </c>
       <c r="F2" s="24"/>
       <c r="G2" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H2" s="22"/>
     </row>
@@ -920,7 +920,7 @@
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H4" s="23"/>
     </row>
@@ -1025,7 +1025,7 @@
         <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1094,11 +1094,11 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1124,7 +1124,7 @@
       <c r="B25" s="9">
         <v>15</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="17" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1161,11 +1161,11 @@
     </row>
     <row r="29" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1192,11 +1192,11 @@
     </row>
     <row r="32" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1223,11 +1223,11 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1254,11 +1254,11 @@
     </row>
     <row r="38" spans="1:3" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1285,11 +1285,11 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="21" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Tutorati pronti e serviti
</commit_message>
<xml_diff>
--- a/UniPD/Tutor Didattico/Automi - Semestre 2/Calendario_ALF_2024_Aggiornato_Tutorati.xlsx
+++ b/UniPD/Tutor Didattico/Automi - Semestre 2/Calendario_ALF_2024_Aggiornato_Tutorati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roves\OneDrive\Documenti\GitHub\Teaching-And-Tutoring\UniPD\Tutor Didattico\Automi - Semestre 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FE475B-91E7-41CC-95D6-934629BD5C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060C5CE7-691D-4BBA-AE36-4CB7165070B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7C55FAAF-9703-2848-805D-6B612CD4CF68}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7C55FAAF-9703-2848-805D-6B612CD4CF68}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendario" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>Il pumping lemma. Linguaggi non regolari</t>
   </si>
@@ -273,16 +273,13 @@
     <t>Vacanze di Pasqua (29/03-02/04)</t>
   </si>
   <si>
-    <t>Orario di tutorato possibile: 12:30/14:30</t>
-  </si>
-  <si>
-    <t>Aula possibile: Luf2 / 1BC50</t>
-  </si>
-  <si>
     <t>Tutorato 10 07/06</t>
   </si>
   <si>
     <t>Tutorato 5 18/04</t>
+  </si>
+  <si>
+    <t>Orario di tutorato : 14:30/16:30</t>
   </si>
 </sst>
 </file>
@@ -344,7 +341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -432,6 +429,37 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -506,41 +534,47 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -858,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B68855-53FD-474B-AE0F-2554AA20AC8B}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:C24"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -867,6 +901,7 @@
     <col min="1" max="1" width="16.19921875" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.09765625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.796875" customWidth="1"/>
+    <col min="8" max="8" width="20.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -887,14 +922,14 @@
       <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="22"/>
+      <c r="F2" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="34"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
@@ -903,10 +938,10 @@
       <c r="B3" s="20">
         <v>2</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="28"/>
+      <c r="C3" s="25"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
@@ -915,14 +950,11 @@
       <c r="B4" s="5">
         <v>3</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="23"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
@@ -931,7 +963,7 @@
       <c r="B5" s="20">
         <v>4</v>
       </c>
-      <c r="C5" s="34"/>
+      <c r="C5" s="27"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
@@ -949,7 +981,7 @@
       <c r="B7" s="5">
         <v>5</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="26" t="s">
         <v>7</v>
       </c>
     </row>
@@ -960,7 +992,7 @@
       <c r="B8" s="6">
         <v>6</v>
       </c>
-      <c r="C8" s="35"/>
+      <c r="C8" s="28"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
@@ -978,7 +1010,7 @@
       <c r="B10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="26" t="s">
         <v>0</v>
       </c>
     </row>
@@ -989,7 +1021,7 @@
       <c r="B11" s="6">
         <v>8</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="28"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
@@ -1094,7 +1126,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="15" t="s">
@@ -1106,7 +1138,7 @@
         <v>43</v>
       </c>
       <c r="B23" s="6"/>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="22" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1115,7 +1147,7 @@
         <v>44</v>
       </c>
       <c r="B24" s="6"/>
-      <c r="C24" s="30"/>
+      <c r="C24" s="23"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
@@ -1285,7 +1317,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="15" t="s">
@@ -1297,7 +1329,7 @@
         <v>56</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="29" t="s">
+      <c r="C42" s="22" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1306,7 +1338,7 @@
         <v>58</v>
       </c>
       <c r="B43" s="6"/>
-      <c r="C43" s="30"/>
+      <c r="C43" s="23"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="11"/>
@@ -1315,7 +1347,8 @@
       <c r="A45" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="F2:H3"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="C2:C3"/>

</xml_diff>

<commit_message>
Some changes here and there
</commit_message>
<xml_diff>
--- a/UniPD/Tutor Didattico/Automi - Semestre 2/Calendario_ALF_2024_Aggiornato_Tutorati.xlsx
+++ b/UniPD/Tutor Didattico/Automi - Semestre 2/Calendario_ALF_2024_Aggiornato_Tutorati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roves\OneDrive\Documenti\GitHub\Teaching-And-Tutoring\UniPD\Tutor Didattico\Automi - Semestre 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060C5CE7-691D-4BBA-AE36-4CB7165070B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F639B8-1F99-480F-98BC-F844D6EE0051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7C55FAAF-9703-2848-805D-6B612CD4CF68}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{7C55FAAF-9703-2848-805D-6B612CD4CF68}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendario" sheetId="1" r:id="rId1"/>
@@ -534,6 +534,27 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -554,27 +575,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -892,7 +892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B68855-53FD-474B-AE0F-2554AA20AC8B}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:H3"/>
     </sheetView>
   </sheetViews>
@@ -922,14 +922,14 @@
       <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="35"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
@@ -938,10 +938,10 @@
       <c r="B3" s="20">
         <v>2</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
@@ -950,11 +950,11 @@
       <c r="B4" s="5">
         <v>3</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
@@ -963,7 +963,7 @@
       <c r="B5" s="20">
         <v>4</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="34"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
@@ -981,7 +981,7 @@
       <c r="B7" s="5">
         <v>5</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="33" t="s">
         <v>7</v>
       </c>
     </row>
@@ -992,7 +992,7 @@
       <c r="B8" s="6">
         <v>6</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="35"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
@@ -1010,7 +1010,7 @@
       <c r="B10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="33" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1021,7 +1021,7 @@
       <c r="B11" s="6">
         <v>8</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="35"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
@@ -1138,7 +1138,7 @@
         <v>43</v>
       </c>
       <c r="B23" s="6"/>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="29" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1147,7 +1147,7 @@
         <v>44</v>
       </c>
       <c r="B24" s="6"/>
-      <c r="C24" s="23"/>
+      <c r="C24" s="30"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
@@ -1329,7 +1329,7 @@
         <v>56</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="22" t="s">
+      <c r="C42" s="29" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1338,7 +1338,7 @@
         <v>58</v>
       </c>
       <c r="B43" s="6"/>
-      <c r="C43" s="23"/>
+      <c r="C43" s="30"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="11"/>

</xml_diff>